<commit_message>
- add column ViTriKho
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhMucHangHoa.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhMucHangHoa.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Trạng thái</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Vị trí kho</t>
   </si>
 </sst>
 </file>
@@ -99,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +117,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,26 +237,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -555,43 +564,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="9" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="4" width="22.85546875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="9" customWidth="1"/>
+    <col min="9" max="10" width="15.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="3" spans="1:11" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="3" spans="1:12" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -602,336 +612,364 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="8"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="6"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="8"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="6"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="8"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="6"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="8"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="8"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="8"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="8"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="8"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="8"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="8"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="8"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="8"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="8"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="6"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="8"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="8"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="6"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="8"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="8"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="2"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="8"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="8"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="8"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="8"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="8"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="8"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="8"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="8"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="J27" s="8"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="12">
-        <f>SUM($H$4:H27)</f>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="16">
+        <f>SUM($I$4:I27)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="11"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A28:H28"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>